<commit_message>
Added code for ST to ROM, implemented the circuit for SRCTOM, adjusted xlsx file accordingly
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23017"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9A7AD6E-7F7E-466F-BC88-2CF02B228048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28785" windowHeight="12840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>3-Bits</t>
   </si>
@@ -166,7 +152,7 @@
     <t>M[AR] &lt;- DST</t>
   </si>
   <si>
-    <t>DSTTOM</t>
+    <t>SRCTOM</t>
   </si>
   <si>
     <t>RESERVED???</t>
@@ -212,6 +198,30 @@
   </si>
   <si>
     <t>ST</t>
+  </si>
+  <si>
+    <t>BINARY EQ.</t>
+  </si>
+  <si>
+    <t>HEX EQ.</t>
+  </si>
+  <si>
+    <t>OFFSET ADDR:</t>
+  </si>
+  <si>
+    <t>NOPE</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>e00048</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>FETCH</t>
   </si>
   <si>
     <t>MOVE:</t>
@@ -223,8 +233,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -237,8 +253,159 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,12 +420,204 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -266,92 +625,384 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF70AD47"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="0070AD47"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
       <rgbColor rgb="00003366"/>
       <rgbColor rgb="00339966"/>
       <rgbColor rgb="00003300"/>
@@ -365,9 +1016,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -416,7 +1064,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -449,26 +1097,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -501,23 +1132,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -659,33 +1273,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G3:O49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="G3:V49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:I7"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.24761904761905" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="8" max="8" width="14.8761904761905" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="13" max="13" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="15.375" customWidth="1"/>
-    <col min="18" max="18" width="22.75" customWidth="1"/>
+    <col min="13" max="13" width="12.6285714285714" customWidth="1"/>
+    <col min="14" max="14" width="15.3714285714286" customWidth="1"/>
+    <col min="18" max="18" width="22.752380952381" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="7:15">
+    <row r="3" spans="8:14">
       <c r="H3" t="s">
         <v>0</v>
       </c>
@@ -696,7 +1305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="7:15">
+    <row r="4" spans="8:14">
       <c r="H4" t="s">
         <v>1</v>
       </c>
@@ -707,7 +1316,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="7:15">
+    <row r="5" spans="7:14">
       <c r="G5">
         <v>0</v>
       </c>
@@ -727,7 +1336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="7:15" ht="13.9">
+    <row r="6" spans="7:15">
       <c r="G6">
         <v>1</v>
       </c>
@@ -756,14 +1365,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="7:15" ht="13.9">
+    <row r="7" spans="7:15">
       <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J7">
@@ -785,11 +1394,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="7:15" ht="13.9">
+    <row r="8" spans="7:13">
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I8" t="s">
@@ -808,7 +1417,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="7:15">
+    <row r="9" spans="7:13">
       <c r="G9">
         <v>4</v>
       </c>
@@ -831,7 +1440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="7:15">
+    <row r="10" spans="7:13">
       <c r="G10">
         <v>5</v>
       </c>
@@ -854,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="7:15">
+    <row r="11" spans="7:13">
       <c r="G11">
         <v>6</v>
       </c>
@@ -877,14 +1486,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="7:15">
+    <row r="12" spans="7:13">
       <c r="G12">
         <v>7</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="J12">
@@ -897,71 +1506,67 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="8:15">
-      <c r="I19" t="s">
+    <row r="19" spans="9:15">
+      <c r="I19" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="8:15" ht="13.9">
-      <c r="I20">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="9:15">
+      <c r="I20" s="4">
         <v>3</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="4">
         <v>3</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="4">
         <v>3</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="4">
         <v>2</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="4">
         <v>2</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>8</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="8:15" ht="13.9">
-      <c r="I21" t="s">
+    <row r="21" spans="9:15">
+      <c r="I21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N21" t="s">
+      <c r="N21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="8:15">
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="8:15" ht="13.9">
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="8:15" ht="13.9"/>
-    <row r="27" spans="8:15" ht="13.9"/>
-    <row r="28" spans="8:15" ht="13.9"/>
-    <row r="29" spans="8:15" ht="13.9">
+    <row r="29" spans="7:13">
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
       <c r="H29" t="s">
         <v>37</v>
       </c>
@@ -978,8 +1583,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="8:15" ht="13.9"/>
-    <row r="31" spans="8:15" ht="13.9">
+    <row r="31" spans="7:9">
+      <c r="G31">
+        <v>0</v>
+      </c>
       <c r="H31" t="s">
         <v>42</v>
       </c>
@@ -987,7 +1594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="8:15" ht="13.9">
+    <row r="32" spans="8:13">
       <c r="H32">
         <v>0</v>
       </c>
@@ -1007,7 +1614,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="8:13" ht="13.9">
+    <row r="33" spans="8:13">
       <c r="H33">
         <v>0</v>
       </c>
@@ -1027,7 +1634,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="8:13" ht="13.9">
+    <row r="34" spans="8:12">
       <c r="H34">
         <v>0</v>
       </c>
@@ -1044,8 +1651,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="8:13" ht="13.9"/>
-    <row r="37" spans="8:13" ht="13.9">
+    <row r="37" spans="7:9">
+      <c r="G37">
+        <v>4</v>
+      </c>
       <c r="H37" t="s">
         <v>45</v>
       </c>
@@ -1053,14 +1662,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="8:13" ht="13.9">
+    <row r="38" spans="8:13">
       <c r="H38">
         <v>10</v>
       </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="3">
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
         <v>0</v>
       </c>
       <c r="K38">
@@ -1073,7 +1682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="8:13" ht="13.9">
+    <row r="39" spans="8:13">
       <c r="H39">
         <v>11</v>
       </c>
@@ -1093,7 +1702,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="8:13" ht="13.9">
+    <row r="40" spans="8:13">
       <c r="H40">
         <v>0</v>
       </c>
@@ -1113,21 +1722,121 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="8:13" ht="13.9"/>
-    <row r="42" spans="8:13" ht="13.9">
+    <row r="42" spans="7:22">
+      <c r="G42">
+        <v>8</v>
+      </c>
       <c r="H42" t="s">
         <v>48</v>
       </c>
       <c r="I42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="8:13">
+      <c r="N42" t="s">
+        <v>50</v>
+      </c>
+      <c r="U42" t="s">
+        <v>51</v>
+      </c>
+      <c r="V42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="8:22">
+      <c r="H43" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" t="s">
+        <v>53</v>
+      </c>
+      <c r="J43" t="s">
+        <v>53</v>
+      </c>
+      <c r="K43" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" t="s">
+        <v>54</v>
+      </c>
+      <c r="M43" t="s">
+        <v>44</v>
+      </c>
+      <c r="N43">
+        <v>7</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <v>0</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>9</v>
+      </c>
+      <c r="U43" t="s">
+        <v>55</v>
+      </c>
+      <c r="V43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="8:21">
+      <c r="H44" t="s">
+        <v>53</v>
+      </c>
+      <c r="I44" t="s">
+        <v>53</v>
+      </c>
+      <c r="J44" t="s">
+        <v>53</v>
+      </c>
+      <c r="K44" t="s">
+        <v>43</v>
+      </c>
+      <c r="L44" t="s">
+        <v>56</v>
+      </c>
+      <c r="M44" t="s">
+        <v>57</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44"/>
+      <c r="U44">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9">
+      <c r="G47">
+        <v>12</v>
+      </c>
       <c r="H47" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="I47" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="8:13">
@@ -1171,7 +1880,41 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{c1ed4991-92b1-418a-93c4-f5c99e7495b5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{c1ed4991-92b1-418a-93c4-f5c99e7495b5}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a sample program to test MOV, LD and ST operations into xlsx file
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>3-Bits</t>
   </si>
@@ -28,9 +28,18 @@
     <t>F3</t>
   </si>
   <si>
+    <t>CODE SAMPLES</t>
+  </si>
+  <si>
+    <t>HEX FORMAT</t>
+  </si>
+  <si>
     <t>Nope</t>
   </si>
   <si>
+    <t>#code that writes 64 into 64th memory cell</t>
+  </si>
+  <si>
     <t>DST &lt;- SRC</t>
   </si>
   <si>
@@ -49,6 +58,12 @@
     <t>MARTIRL</t>
   </si>
   <si>
+    <t>LD R0 IM 64</t>
+  </si>
+  <si>
+    <t>40 00</t>
+  </si>
+  <si>
     <t>DST &lt;- M[AR]</t>
   </si>
   <si>
@@ -65,6 +80,12 @@
   </si>
   <si>
     <t>MARTIRH</t>
+  </si>
+  <si>
+    <t>MOV AR R0</t>
+  </si>
+  <si>
+    <t>00 16</t>
   </si>
   <si>
     <r>
@@ -87,24 +108,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-      </rPr>
-      <t>IRTO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t>DST</t>
-    </r>
+    <t>IRTODST</t>
   </si>
   <si>
     <t>RF1 &lt;- RF1 | RF2</t>
@@ -113,6 +117,12 @@
     <t>OR</t>
   </si>
   <si>
+    <t>ST RO D</t>
+  </si>
+  <si>
+    <t>00 09</t>
+  </si>
+  <si>
     <t>SRC &lt;- SRC + 1</t>
   </si>
   <si>
@@ -159,6 +169,12 @@
   </si>
   <si>
     <t>Format</t>
+  </si>
+  <si>
+    <t>BIT SIZE</t>
+  </si>
+  <si>
+    <t>SYMBOLS</t>
   </si>
   <si>
     <t>F1</t>
@@ -240,7 +256,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -252,6 +268,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -728,152 +750,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -888,6 +910,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
@@ -1279,10 +1307,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="G3:V49"/>
+  <dimension ref="G3:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.24761904761905" defaultRowHeight="15"/>
@@ -1292,6 +1320,7 @@
     <col min="13" max="13" width="12.6285714285714" customWidth="1"/>
     <col min="14" max="14" width="15.3714285714286" customWidth="1"/>
     <col min="18" max="18" width="22.752380952381" customWidth="1"/>
+    <col min="22" max="22" width="30.6095238095238" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="8:14">
@@ -1305,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="8:14">
+    <row r="4" spans="8:24">
       <c r="H4" t="s">
         <v>1</v>
       </c>
@@ -1315,106 +1344,133 @@
       <c r="N4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="7:14">
+      <c r="V4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="7:22">
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="7:15">
+        <v>6</v>
+      </c>
+      <c r="V5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="7:24">
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="7:15">
+        <v>13</v>
+      </c>
+      <c r="V6" t="s">
+        <v>14</v>
+      </c>
+      <c r="X6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="7:24">
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J7">
         <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="L7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="M7">
         <v>2</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="7:13">
+        <v>21</v>
+      </c>
+      <c r="V7" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="7:24">
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M8">
         <v>3</v>
+      </c>
+      <c r="V8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="7:13">
@@ -1422,19 +1478,19 @@
         <v>4</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="J9">
         <v>4</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="M9">
         <v>4</v>
@@ -1445,19 +1501,19 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="M10">
         <v>5</v>
@@ -1468,19 +1524,19 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="J11">
         <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -1491,33 +1547,39 @@
         <v>7</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="J12">
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="M12">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="9:15">
-      <c r="I19" s="4" t="s">
-        <v>36</v>
-      </c>
+    <row r="19" spans="8:14">
+      <c r="H19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="9:15">
+    </row>
+    <row r="20" spans="7:14">
+      <c r="G20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="4">
+        <v>3</v>
+      </c>
       <c r="I20" s="4">
         <v>3</v>
       </c>
@@ -1525,93 +1587,70 @@
         <v>3</v>
       </c>
       <c r="K20" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L20" s="4">
         <v>2</v>
       </c>
       <c r="M20" s="4">
+        <v>8</v>
+      </c>
+      <c r="N20" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14">
+      <c r="G21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N20" s="4">
-        <v>8</v>
-      </c>
-      <c r="O20" s="4">
+      <c r="J21" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="9:15">
-      <c r="I21" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="4" t="s">
+      <c r="K21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="8:13">
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" t="s">
         <v>2</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="7:13">
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" t="s">
-        <v>37</v>
       </c>
       <c r="J29" t="s">
         <v>3</v>
       </c>
       <c r="K29" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="L29" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="M29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="7:9">
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="8:13">
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="K32" t="s">
-        <v>43</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32" t="s">
-        <v>44</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="8:13">
@@ -1622,32 +1661,52 @@
         <v>0</v>
       </c>
       <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>54</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="8:13">
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>10</v>
       </c>
-      <c r="K33" t="s">
-        <v>43</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="8:12">
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="8:12">
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>54</v>
+      </c>
+      <c r="L35">
         <v>11</v>
       </c>
     </row>
@@ -1656,20 +1715,20 @@
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I37" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="8:13">
       <c r="H38">
         <v>10</v>
       </c>
-      <c r="I38" s="5">
-        <v>0</v>
-      </c>
-      <c r="J38" s="5">
+      <c r="I38" s="7">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7">
         <v>0</v>
       </c>
       <c r="K38">
@@ -1679,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="8:13">
@@ -1699,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="8:13">
@@ -1727,39 +1786,39 @@
         <v>8</v>
       </c>
       <c r="H42" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="I42" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="N42" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="U42" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="V42" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="8:22">
       <c r="H43" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I43" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J43" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="K43" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="L43" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="M43" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="N43">
         <v>7</v>
@@ -1780,7 +1839,7 @@
         <v>9</v>
       </c>
       <c r="U43" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="V43">
         <v>8</v>
@@ -1788,22 +1847,22 @@
     </row>
     <row r="44" spans="8:21">
       <c r="H44" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="I44" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J44" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="K44" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="L44" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="M44" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -1833,10 +1892,10 @@
         <v>12</v>
       </c>
       <c r="H47" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="I47" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="8:13">
@@ -1856,7 +1915,7 @@
         <v>0</v>
       </c>
       <c r="M48" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="8:13">
@@ -1889,7 +1948,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{c1ed4991-92b1-418a-93c4-f5c99e7495b5}</x14:id>
+          <x14:id>{567a05a1-c0f5-4aab-8f85-9c96d4409e68}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -1901,7 +1960,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{c1ed4991-92b1-418a-93c4-f5c99e7495b5}">
+          <x14:cfRule type="dataBar" id="{567a05a1-c0f5-4aab-8f85-9c96d4409e68}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
stack mo's and ir[L] to src done
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20361"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ekrem\Desktop\corg-final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF3D4B4-B197-462C-BC04-75F666395E3B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28785" windowHeight="12840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>3-Bits</t>
   </si>
@@ -245,18 +251,30 @@
   <si>
     <t>MOV</t>
   </si>
+  <si>
+    <t>M[SP] &lt;- SRC</t>
+  </si>
+  <si>
+    <t>SRC &lt;- M[SP]</t>
+  </si>
+  <si>
+    <t>SRCTSP</t>
+  </si>
+  <si>
+    <t>SPTSRC</t>
+  </si>
+  <si>
+    <t>PC &lt;- IR[L]</t>
+  </si>
+  <si>
+    <t>IRLTPC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -276,158 +294,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,169 +321,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -622,24 +333,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="9"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -647,255 +346,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -903,9 +360,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
@@ -920,58 +374,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1044,6 +466,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1301,29 +726,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G3:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.24761904761905" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="14.8761904761905" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="13" max="13" width="12.6285714285714" customWidth="1"/>
-    <col min="14" max="14" width="15.3714285714286" customWidth="1"/>
-    <col min="18" max="18" width="22.752380952381" customWidth="1"/>
-    <col min="22" max="22" width="30.6095238095238" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:14">
+    <row r="3" spans="7:24">
       <c r="H3" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="8:24">
+    <row r="4" spans="7:24">
       <c r="H4" t="s">
         <v>1</v>
       </c>
@@ -1351,7 +776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="7:22">
+    <row r="5" spans="7:24">
       <c r="G5">
         <v>0</v>
       </c>
@@ -1396,10 +821,10 @@
       <c r="M6">
         <v>1</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="9" t="s">
         <v>13</v>
       </c>
       <c r="V6" t="s">
@@ -1431,10 +856,10 @@
       <c r="M7">
         <v>2</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="V7" t="s">
@@ -1448,10 +873,10 @@
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="J8">
@@ -1466,6 +891,12 @@
       <c r="M8">
         <v>3</v>
       </c>
+      <c r="N8" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>73</v>
+      </c>
       <c r="V8" t="s">
         <v>28</v>
       </c>
@@ -1473,7 +904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="7:13">
+    <row r="9" spans="7:24">
       <c r="G9">
         <v>4</v>
       </c>
@@ -1495,8 +926,14 @@
       <c r="M9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="7:13">
+      <c r="N9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="7:24">
       <c r="G10">
         <v>5</v>
       </c>
@@ -1518,8 +955,14 @@
       <c r="M10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="7:13">
+      <c r="N10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="7:24">
       <c r="G11">
         <v>6</v>
       </c>
@@ -1542,7 +985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="7:13">
+    <row r="12" spans="7:24">
       <c r="G12">
         <v>7</v>
       </c>
@@ -1562,70 +1005,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="8:14">
-      <c r="H19" s="4" t="s">
+    <row r="19" spans="7:14">
+      <c r="H19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="7:14">
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <v>3</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>3</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <v>3</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <v>2</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="3">
         <v>2</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="3">
         <v>8</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="7:14">
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="4" t="s">
+      <c r="N21" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="8:13">
+    <row r="29" spans="7:14">
       <c r="H29" t="s">
         <v>48</v>
       </c>
@@ -1645,7 +1088,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="7:8">
+    <row r="32" spans="7:14">
       <c r="G32">
         <v>0</v>
       </c>
@@ -1653,7 +1096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="8:13">
+    <row r="33" spans="7:22">
       <c r="H33">
         <v>0</v>
       </c>
@@ -1673,7 +1116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="8:13">
+    <row r="34" spans="7:22">
       <c r="H34">
         <v>0</v>
       </c>
@@ -1693,7 +1136,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="8:12">
+    <row r="35" spans="7:22">
       <c r="H35">
         <v>0</v>
       </c>
@@ -1710,7 +1153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="7:9">
+    <row r="37" spans="7:22">
       <c r="G37">
         <v>4</v>
       </c>
@@ -1721,14 +1164,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="8:13">
+    <row r="38" spans="7:22">
       <c r="H38">
         <v>10</v>
       </c>
-      <c r="I38" s="7">
-        <v>0</v>
-      </c>
-      <c r="J38" s="7">
+      <c r="I38" s="6">
+        <v>0</v>
+      </c>
+      <c r="J38" s="6">
         <v>0</v>
       </c>
       <c r="K38">
@@ -1741,7 +1184,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="8:13">
+    <row r="39" spans="7:22">
       <c r="H39">
         <v>11</v>
       </c>
@@ -1761,7 +1204,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="8:13">
+    <row r="40" spans="7:22">
       <c r="H40">
         <v>0</v>
       </c>
@@ -1801,7 +1244,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="8:22">
+    <row r="43" spans="7:22">
       <c r="H43" t="s">
         <v>43</v>
       </c>
@@ -1845,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="8:21">
+    <row r="44" spans="7:22">
       <c r="H44" t="s">
         <v>64</v>
       </c>
@@ -1882,12 +1325,11 @@
       <c r="S44">
         <v>0</v>
       </c>
-      <c r="T44"/>
       <c r="U44">
         <v>800</v>
       </c>
     </row>
-    <row r="47" spans="7:9">
+    <row r="47" spans="7:22">
       <c r="G47">
         <v>12</v>
       </c>
@@ -1898,7 +1340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="8:13">
+    <row r="48" spans="7:22">
       <c r="H48">
         <v>1</v>
       </c>
@@ -1948,19 +1390,18 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{567a05a1-c0f5-4aab-8f85-9c96d4409e68}</x14:id>
+          <x14:id>{567A05A1-C0F5-4AAB-8F85-9C96D4409E68}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{567a05a1-c0f5-4aab-8f85-9c96d4409e68}">
+          <x14:cfRule type="dataBar" id="{567A05A1-C0F5-4AAB-8F85-9C96D4409E68}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>

<commit_message>
benim bitti heralde size kg
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
   <si>
     <t>3-Bits</t>
   </si>
@@ -34,6 +34,9 @@
     <t>HEX FORMAT</t>
   </si>
   <si>
+    <t>INC R0</t>
+  </si>
+  <si>
     <t>DST &lt;- SRC</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>#code that writes 64 into 64th memory cell</t>
+  </si>
+  <si>
+    <t>00 40</t>
   </si>
   <si>
     <t>DST &lt;- M[AR]</t>
@@ -191,6 +197,9 @@
     <t>#circular negation</t>
   </si>
   <si>
+    <t>#circular lssrc</t>
+  </si>
+  <si>
     <t>INC R1 R0</t>
   </si>
   <si>
@@ -203,6 +212,12 @@
     <t>00 59</t>
   </si>
   <si>
+    <t>LSL R1 R0</t>
+  </si>
+  <si>
+    <t>00 61</t>
+  </si>
+  <si>
     <t>INC AR R1</t>
   </si>
   <si>
@@ -215,6 +230,12 @@
     <t>20 5e</t>
   </si>
   <si>
+    <t>LSL AR R1</t>
+  </si>
+  <si>
+    <t>20 66</t>
+  </si>
+  <si>
     <t>Format</t>
   </si>
   <si>
@@ -230,6 +251,12 @@
     <t>c0 5f</t>
   </si>
   <si>
+    <t>LSL SP AR</t>
+  </si>
+  <si>
+    <t>c0 67</t>
+  </si>
+  <si>
     <t>BIT SIZE</t>
   </si>
   <si>
@@ -243,6 +270,12 @@
   </si>
   <si>
     <t>e0 5a</t>
+  </si>
+  <si>
+    <t>LSL R2 SP</t>
+  </si>
+  <si>
+    <t>e0 62</t>
   </si>
   <si>
     <t>SYMBOLS</t>
@@ -318,11 +351,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font/>
   </fonts>
   <fills count="4">
     <fill>
@@ -442,6 +475,9 @@
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -450,6 +486,9 @@
     </xf>
     <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -460,13 +499,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -760,291 +793,318 @@
       <c r="O3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="R3" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>1.0</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7">
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8">
         <v>1.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6">
         <v>1.0</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="I4" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="M4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
+      <c r="R4" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>2.0</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
         <v>2.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="5">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6">
         <v>2.0</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>19</v>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>3.0</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="8">
         <v>3.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="5">
+        <v>27</v>
+      </c>
+      <c r="G6" s="6">
         <v>3.0</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>27</v>
+      <c r="H6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>4.0</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
         <v>4.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="5">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6">
         <v>4.0</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>35</v>
+      <c r="H7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
         <v>5.0</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>39</v>
+      <c r="B8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D8" s="1">
         <v>5.0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1">
         <v>5.0</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>43</v>
+      <c r="H8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
         <v>6.0</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>45</v>
+      <c r="B9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>6.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G9" s="1">
         <v>6.0</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>48</v>
+      <c r="H9" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>7.0</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="8">
         <v>7.0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>7.0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q10" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="M10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11">
-      <c r="M11" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="S11" s="11" t="s">
+      <c r="M11" s="9" t="s">
         <v>60</v>
       </c>
+      <c r="O11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12">
-      <c r="M12" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="O12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q12" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>64</v>
+      <c r="M12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="O13" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q13" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T13" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C14" s="13">
         <v>3.0</v>
@@ -1067,25 +1127,31 @@
       <c r="I14" s="13">
         <v>3.0</v>
       </c>
-      <c r="M14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q14" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>74</v>
+      <c r="M14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="T14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="13" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>2</v>
@@ -1094,24 +1160,24 @@
         <v>3</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>82</v>
+      <c r="A17" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -1142,7 +1208,7 @@
         <v>1.0</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -1236,8 +1302,8 @@
       <c r="H22" s="14">
         <v>0.0</v>
       </c>
-      <c r="J22" s="10" t="s">
-        <v>84</v>
+      <c r="J22" s="12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -1321,8 +1387,8 @@
       <c r="H26" s="14">
         <v>0.0</v>
       </c>
-      <c r="J26" s="10" t="s">
-        <v>85</v>
+      <c r="J26" s="12" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -1388,8 +1454,8 @@
       <c r="H30" s="14">
         <v>0.0</v>
       </c>
-      <c r="J30" s="10" t="s">
-        <v>86</v>
+      <c r="J30" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1461,8 +1527,8 @@
       <c r="H34" s="13">
         <v>10001.0</v>
       </c>
-      <c r="J34" s="10" t="s">
-        <v>87</v>
+      <c r="J34" s="12" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -1489,7 +1555,7 @@
       <c r="G35" s="13">
         <v>0.0</v>
       </c>
-      <c r="H35" s="12">
+      <c r="H35" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -1540,8 +1606,8 @@
       <c r="H38" s="13">
         <v>10101.0</v>
       </c>
-      <c r="J38" s="10" t="s">
-        <v>88</v>
+      <c r="J38" s="12" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -1568,7 +1634,7 @@
       <c r="G39" s="13">
         <v>0.0</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -1619,8 +1685,8 @@
       <c r="H42" s="13">
         <v>11001.0</v>
       </c>
-      <c r="J42" s="10" t="s">
-        <v>10</v>
+      <c r="J42" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -1647,7 +1713,7 @@
       <c r="G43" s="13">
         <v>0.0</v>
       </c>
-      <c r="H43" s="12">
+      <c r="H43" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -1698,8 +1764,8 @@
       <c r="H46" s="13">
         <v>11101.0</v>
       </c>
-      <c r="J46" s="10" t="s">
-        <v>39</v>
+      <c r="J46" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -1726,7 +1792,7 @@
       <c r="G47" s="13">
         <v>0.0</v>
       </c>
-      <c r="H47" s="12">
+      <c r="H47" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -1777,8 +1843,8 @@
       <c r="H50" s="1">
         <v>100001.0</v>
       </c>
-      <c r="J50" s="10" t="s">
-        <v>45</v>
+      <c r="J50" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -1857,8 +1923,8 @@
         <v>100101.0</v>
       </c>
       <c r="I54" s="1"/>
-      <c r="J54" s="10" t="s">
-        <v>31</v>
+      <c r="J54" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -1946,8 +2012,8 @@
         <v>101001.0</v>
       </c>
       <c r="I58" s="1"/>
-      <c r="J58" s="10" t="s">
-        <v>17</v>
+      <c r="J58" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -2045,8 +2111,8 @@
       <c r="H62" s="1">
         <v>101101.0</v>
       </c>
-      <c r="J62" s="10" t="s">
-        <v>25</v>
+      <c r="J62" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -2073,7 +2139,7 @@
       <c r="G63" s="13">
         <v>0.0</v>
       </c>
-      <c r="H63" s="12">
+      <c r="H63" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2121,11 +2187,11 @@
       <c r="G66" s="13">
         <v>0.0</v>
       </c>
-      <c r="H66" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>33</v>
+      <c r="H66" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J66" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -2182,11 +2248,11 @@
       <c r="G70" s="13">
         <v>0.0</v>
       </c>
-      <c r="H70" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="J70" s="10" t="s">
-        <v>89</v>
+      <c r="H70" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J70" s="12" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -2243,11 +2309,11 @@
       <c r="G74" s="13">
         <v>0.0</v>
       </c>
-      <c r="H74" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="J74" s="10" t="s">
-        <v>90</v>
+      <c r="H74" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J74" s="12" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -2307,8 +2373,8 @@
       <c r="H78" s="13">
         <v>111101.0</v>
       </c>
-      <c r="J78" s="10" t="s">
-        <v>91</v>
+      <c r="J78" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
@@ -2386,8 +2452,8 @@
       <c r="H82" s="13">
         <v>1000010.0</v>
       </c>
-      <c r="J82" s="10" t="s">
-        <v>92</v>
+      <c r="J82" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -2417,7 +2483,7 @@
       <c r="H83" s="13">
         <v>0.0</v>
       </c>
-      <c r="J83" s="10"/>
+      <c r="J83" s="12"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="13" t="str">
@@ -2443,10 +2509,10 @@
       <c r="G84" s="13">
         <v>0.0</v>
       </c>
-      <c r="H84" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="J84" s="10"/>
+      <c r="H84" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J84" s="12"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="13" t="str">
@@ -2457,7 +2523,7 @@
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="J85" s="10"/>
+      <c r="J85" s="12"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="13" t="str">
@@ -2483,11 +2549,11 @@
       <c r="G86" s="13">
         <v>0.0</v>
       </c>
-      <c r="H86" s="12">
-        <v>0.0</v>
-      </c>
-      <c r="J86" s="10" t="s">
-        <v>93</v>
+      <c r="H86" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="J86" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
@@ -2499,7 +2565,7 @@
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="J87" s="10"/>
+      <c r="J87" s="12"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="13" t="str">
@@ -2510,7 +2576,7 @@
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="J88" s="10"/>
+      <c r="J88" s="12"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="13" t="str">
@@ -2521,7 +2587,7 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="J89" s="10"/>
+      <c r="J89" s="12"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="13" t="str">
@@ -2550,8 +2616,8 @@
       <c r="H90" s="13">
         <v>1001001.0</v>
       </c>
-      <c r="J90" s="10" t="s">
-        <v>94</v>
+      <c r="J90" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
@@ -2606,7 +2672,7 @@
       <c r="G92" s="13">
         <v>0.0</v>
       </c>
-      <c r="H92" s="12">
+      <c r="H92" s="5">
         <v>0.0</v>
       </c>
     </row>
@@ -2647,8 +2713,8 @@
       <c r="H94" s="13">
         <v>1001101.0</v>
       </c>
-      <c r="J94" s="10" t="s">
-        <v>95</v>
+      <c r="J94" s="12" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
@@ -2675,7 +2741,7 @@
       <c r="G95" s="13">
         <v>0.0</v>
       </c>
-      <c r="H95" s="12">
+      <c r="H95" s="5">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pul, push, call and ret examples
</commit_message>
<xml_diff>
--- a/format.xlsx
+++ b/format.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ekrem\Desktop\corg-final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DB07F5-4F46-42DD-B9E9-584CEAB5318D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="148">
   <si>
     <t>3-Bits</t>
   </si>
@@ -467,23 +476,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -498,7 +494,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +505,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -785,126 +787,129 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="40">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -915,26 +920,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff70ad47"/>
-      <rgbColor rgb="ff006100"/>
-      <rgbColor rgb="ff598a38"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF70AD47"/>
+      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF598A38"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1136,7 +1200,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1155,7 +1219,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1185,7 +1249,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1211,7 +1275,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1237,7 +1301,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1327,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1289,7 +1353,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1315,7 +1379,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1341,7 +1405,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1367,7 +1431,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1393,7 +1457,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1406,9 +1470,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1425,7 +1495,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1444,7 +1514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1470,7 +1540,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1496,7 +1566,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1522,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1548,7 +1618,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1574,7 +1644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1600,7 +1670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1626,7 +1696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1652,7 +1722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1678,7 +1748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1691,9 +1761,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1707,7 +1783,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1726,7 +1802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1756,7 +1832,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1782,7 +1858,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1808,7 +1884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1834,7 +1910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1860,7 +1936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1886,7 +1962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1912,7 +1988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1938,7 +2014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1964,7 +2040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1977,49 +2053,59 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V97"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E76" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.67188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8516" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.67188" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3516" style="1" customWidth="1"/>
-    <col min="6" max="7" width="8.67188" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6719" style="1" customWidth="1"/>
-    <col min="9" max="14" width="8.67188" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.1719" style="1" customWidth="1"/>
-    <col min="16" max="22" width="8.67188" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="1" customWidth="1"/>
+    <col min="16" max="22" width="8.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
+    <row r="1" spans="1:22" ht="13.5" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" t="s" s="3">
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2"/>
@@ -2037,19 +2123,19 @@
       <c r="U1" s="4"/>
       <c r="V1" s="5"/>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
+    <row r="2" spans="1:22" ht="13.5" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="2"/>
@@ -2067,41 +2153,41 @@
       <c r="U2" s="2"/>
       <c r="V2" s="6"/>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
+    <row r="3" spans="1:22" ht="13.5" customHeight="1">
       <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="7">
         <v>0</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" t="s" s="8">
+      <c r="H3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" t="s" s="3">
+      <c r="M3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="N3" s="2"/>
-      <c r="O3" t="s" s="3">
+      <c r="O3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" t="s" s="3">
+      <c r="R3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="S3" s="2"/>
@@ -2109,45 +2195,45 @@
       <c r="U3" s="2"/>
       <c r="V3" s="6"/>
     </row>
-    <row r="4" ht="14.65" customHeight="1">
+    <row r="4" spans="1:22" ht="14.65" customHeight="1">
       <c r="A4" s="10">
         <v>1</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" t="s" s="13">
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s" s="13">
+      <c r="F4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
       </c>
-      <c r="H4" t="s" s="11">
+      <c r="H4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s" s="11">
+      <c r="I4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" t="s" s="3">
+      <c r="M4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" t="s" s="15">
+      <c r="R4" s="15" t="s">
         <v>15</v>
       </c>
       <c r="S4" s="2"/>
@@ -2155,42 +2241,42 @@
       <c r="U4" s="2"/>
       <c r="V4" s="6"/>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
+    <row r="5" spans="1:22" ht="13.5" customHeight="1">
       <c r="A5" s="10">
         <v>2</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="12">
         <v>2</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="10">
         <v>2</v>
       </c>
-      <c r="H5" t="s" s="11">
+      <c r="H5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="s" s="11">
+      <c r="I5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" t="s" s="3">
+      <c r="M5" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" t="s" s="3">
+      <c r="O5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="P5" s="2"/>
@@ -2201,42 +2287,42 @@
       <c r="U5" s="2"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
+    <row r="6" spans="1:22" ht="13.5" customHeight="1">
       <c r="A6" s="10">
         <v>3</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="12">
         <v>3</v>
       </c>
-      <c r="E6" t="s" s="13">
+      <c r="E6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s" s="13">
+      <c r="F6" s="13" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="10">
         <v>3</v>
       </c>
-      <c r="H6" t="s" s="11">
+      <c r="H6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I6" t="s" s="11">
+      <c r="I6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" t="s" s="3">
+      <c r="M6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" t="s" s="3">
+      <c r="O6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="P6" s="2"/>
@@ -2247,42 +2333,42 @@
       <c r="U6" s="2"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
+    <row r="7" spans="1:22" ht="13.5" customHeight="1">
       <c r="A7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="12">
         <v>4</v>
       </c>
-      <c r="E7" t="s" s="13">
+      <c r="E7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s" s="13">
+      <c r="F7" s="13" t="s">
         <v>35</v>
       </c>
       <c r="G7" s="10">
         <v>4</v>
       </c>
-      <c r="H7" t="s" s="11">
+      <c r="H7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I7" t="s" s="11">
+      <c r="I7" s="11" t="s">
         <v>37</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" t="s" s="3">
+      <c r="M7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" t="s" s="3">
+      <c r="O7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="P7" s="2"/>
@@ -2293,32 +2379,32 @@
       <c r="U7" s="2"/>
       <c r="V7" s="6"/>
     </row>
-    <row r="8" ht="14.65" customHeight="1">
+    <row r="8" spans="1:22" ht="14.65" customHeight="1">
       <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" t="s" s="16">
+      <c r="B8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s" s="17">
+      <c r="C8" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="E8" t="s" s="13">
+      <c r="E8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s" s="13">
+      <c r="F8" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="7">
         <v>5</v>
       </c>
-      <c r="H8" t="s" s="16">
+      <c r="H8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s" s="16">
+      <c r="I8" s="16" t="s">
         <v>45</v>
       </c>
       <c r="J8" s="2"/>
@@ -2335,32 +2421,32 @@
       <c r="U8" s="2"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
+    <row r="9" spans="1:22" ht="13.5" customHeight="1">
       <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" t="s" s="18">
+      <c r="B9" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s" s="18">
+      <c r="C9" s="18" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="7">
         <v>6</v>
       </c>
-      <c r="E9" t="s" s="13">
+      <c r="E9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F9" t="s" s="13">
+      <c r="F9" s="13" t="s">
         <v>49</v>
       </c>
       <c r="G9" s="7">
         <v>6</v>
       </c>
-      <c r="H9" t="s" s="13">
+      <c r="H9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="I9" t="s" s="13">
+      <c r="I9" s="13" t="s">
         <v>51</v>
       </c>
       <c r="J9" s="2"/>
@@ -2368,7 +2454,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" t="s" s="3">
+      <c r="O9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P9" s="2"/>
@@ -2379,55 +2465,55 @@
       <c r="U9" s="2"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" ht="14.65" customHeight="1">
+    <row r="10" spans="1:22" ht="14.65" customHeight="1">
       <c r="A10" s="10">
         <v>7</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="C10" s="11" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="12">
         <v>7</v>
       </c>
-      <c r="E10" t="s" s="13">
+      <c r="E10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F10" t="s" s="13">
+      <c r="F10" s="13" t="s">
         <v>55</v>
       </c>
       <c r="G10" s="7">
         <v>7</v>
       </c>
-      <c r="H10" t="s" s="13">
+      <c r="H10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I10" t="s" s="13">
+      <c r="I10" s="13" t="s">
         <v>57</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" t="s" s="15">
+      <c r="M10" s="15" t="s">
         <v>58</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
-      <c r="Q10" t="s" s="15">
+      <c r="Q10" s="15" t="s">
         <v>59</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-      <c r="T10" t="s" s="15">
+      <c r="T10" s="15" t="s">
         <v>60</v>
       </c>
       <c r="U10" s="2"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" ht="14.65" customHeight="1">
+    <row r="11" spans="1:22" ht="14.65" customHeight="1">
       <c r="A11" s="19"/>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -2440,30 +2526,30 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" t="s" s="15">
+      <c r="M11" s="15" t="s">
         <v>61</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" t="s" s="3">
+      <c r="O11" s="3" t="s">
         <v>62</v>
       </c>
       <c r="P11" s="2"/>
-      <c r="Q11" t="s" s="15">
+      <c r="Q11" s="15" t="s">
         <v>63</v>
       </c>
       <c r="R11" s="2"/>
-      <c r="S11" t="s" s="15">
+      <c r="S11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="T11" t="s" s="15">
+      <c r="T11" s="15" t="s">
         <v>65</v>
       </c>
       <c r="U11" s="2"/>
-      <c r="V11" t="s" s="21">
+      <c r="V11" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" ht="14.65" customHeight="1">
+    <row r="12" spans="1:22" ht="14.65" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2476,32 +2562,32 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" t="s" s="15">
+      <c r="M12" s="15" t="s">
         <v>67</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" t="s" s="15">
+      <c r="O12" s="15" t="s">
         <v>68</v>
       </c>
       <c r="P12" s="2"/>
-      <c r="Q12" t="s" s="15">
+      <c r="Q12" s="15" t="s">
         <v>69</v>
       </c>
       <c r="R12" s="2"/>
-      <c r="S12" t="s" s="3">
+      <c r="S12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="T12" t="s" s="15">
+      <c r="T12" s="15" t="s">
         <v>71</v>
       </c>
       <c r="U12" s="2"/>
-      <c r="V12" t="s" s="21">
+      <c r="V12" s="21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" ht="14.65" customHeight="1">
+    <row r="13" spans="1:22" ht="14.65" customHeight="1">
       <c r="A13" s="19"/>
-      <c r="B13" t="s" s="15">
+      <c r="B13" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="2"/>
@@ -2514,32 +2600,32 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" t="s" s="15">
+      <c r="M13" s="15" t="s">
         <v>74</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" t="s" s="15">
+      <c r="O13" s="15" t="s">
         <v>75</v>
       </c>
       <c r="P13" s="2"/>
-      <c r="Q13" t="s" s="15">
+      <c r="Q13" s="15" t="s">
         <v>76</v>
       </c>
       <c r="R13" s="2"/>
-      <c r="S13" t="s" s="3">
+      <c r="S13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="T13" t="s" s="15">
+      <c r="T13" s="15" t="s">
         <v>78</v>
       </c>
       <c r="U13" s="2"/>
-      <c r="V13" t="s" s="21">
+      <c r="V13" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" ht="14.65" customHeight="1">
+    <row r="14" spans="1:22" ht="14.65" customHeight="1">
       <c r="A14" s="19"/>
-      <c r="B14" t="s" s="15">
+      <c r="B14" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C14" s="22">
@@ -2566,53 +2652,53 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" t="s" s="15">
+      <c r="M14" s="15" t="s">
         <v>81</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" t="s" s="15">
+      <c r="O14" s="15" t="s">
         <v>82</v>
       </c>
       <c r="P14" s="2"/>
-      <c r="Q14" t="s" s="15">
+      <c r="Q14" s="15" t="s">
         <v>83</v>
       </c>
       <c r="R14" s="2"/>
-      <c r="S14" t="s" s="3">
+      <c r="S14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="T14" t="s" s="15">
+      <c r="T14" s="15" t="s">
         <v>85</v>
       </c>
       <c r="U14" s="2"/>
-      <c r="V14" t="s" s="21">
+      <c r="V14" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="15" ht="14.65" customHeight="1">
+    <row r="15" spans="1:22" ht="14.65" customHeight="1">
       <c r="A15" s="19"/>
-      <c r="B15" t="s" s="15">
+      <c r="B15" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C15" t="s" s="15">
+      <c r="C15" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D15" t="s" s="15">
+      <c r="D15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s" s="15">
+      <c r="E15" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F15" t="s" s="15">
+      <c r="F15" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G15" t="s" s="15">
+      <c r="G15" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H15" t="s" s="15">
+      <c r="H15" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="I15" t="s" s="15">
+      <c r="I15" s="15" t="s">
         <v>92</v>
       </c>
       <c r="J15" s="2"/>
@@ -2629,7 +2715,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
+    <row r="16" spans="1:22" ht="13.5" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2653,11 +2739,11 @@
       <c r="U16" s="2"/>
       <c r="V16" s="6"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" t="s" s="23">
+    <row r="17" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A17" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B17" t="s" s="3">
+      <c r="B17" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C17" s="2"/>
@@ -2681,12 +2767,12 @@
       <c r="U17" s="2"/>
       <c r="V17" s="6"/>
     </row>
-    <row r="18" ht="14.65" customHeight="1">
-      <c r="A18" s="24">
-        <f>HEX2BIN(B18)</f>
-        <v>0</v>
-      </c>
-      <c r="B18" s="7">
+    <row r="18" spans="1:22" ht="14.65" customHeight="1">
+      <c r="A18" s="24" t="str">
+        <f t="shared" ref="A18:A49" si="0">HEX2BIN(B18)</f>
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="str">
         <f>DEC2HEX(0)</f>
         <v>0</v>
       </c>
@@ -2709,15 +2795,15 @@
         <v>1</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" t="s" s="13">
+      <c r="J18" s="13" t="s">
         <v>95</v>
       </c>
       <c r="K18" s="7">
         <v>8008</v>
       </c>
       <c r="L18" s="2"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -2727,13 +2813,13 @@
       <c r="U18" s="2"/>
       <c r="V18" s="6"/>
     </row>
-    <row r="19" ht="14.65" customHeight="1">
-      <c r="A19" s="24">
-        <f>HEX2BIN(B19)</f>
+    <row r="19" spans="1:22" ht="14.65" customHeight="1">
+      <c r="A19" s="24" t="str">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B19" s="7">
-        <f>DEC2HEX(HEX2DEC(B18)+1)</f>
+      <c r="B19" s="7" t="str">
+        <f t="shared" ref="B19:B50" si="1">DEC2HEX(HEX2DEC(B18)+1)</f>
         <v>1</v>
       </c>
       <c r="C19" s="7">
@@ -2760,14 +2846,14 @@
         <v>10010</v>
       </c>
       <c r="L19" s="2"/>
-      <c r="M19" t="s" s="26">
+      <c r="M19" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="N19" s="25"/>
-      <c r="O19" t="s" s="3">
+      <c r="N19" s="38"/>
+      <c r="O19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P19" t="s" s="3">
+      <c r="P19" s="3" t="s">
         <v>98</v>
       </c>
       <c r="Q19" s="2"/>
@@ -2777,13 +2863,13 @@
       <c r="U19" s="2"/>
       <c r="V19" s="6"/>
     </row>
-    <row r="20" ht="14.65" customHeight="1">
-      <c r="A20" s="24">
-        <f>HEX2BIN(B20)</f>
-        <v>2</v>
-      </c>
-      <c r="B20" s="7">
-        <f>DEC2HEX(HEX2DEC(B19)+1)</f>
+    <row r="20" spans="1:22" ht="14.65" customHeight="1">
+      <c r="A20" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C20" s="7">
@@ -2808,14 +2894,14 @@
         <v>1800</v>
       </c>
       <c r="L20" s="2"/>
-      <c r="M20" t="s" s="26">
+      <c r="M20" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="25"/>
-      <c r="O20" t="s" s="3">
+      <c r="N20" s="38"/>
+      <c r="O20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="P20" t="s" s="3">
+      <c r="P20" s="3" t="s">
         <v>101</v>
       </c>
       <c r="Q20" s="2"/>
@@ -2825,13 +2911,13 @@
       <c r="U20" s="2"/>
       <c r="V20" s="6"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="24">
-        <f>HEX2BIN(B21)</f>
-        <v>3</v>
-      </c>
-      <c r="B21" s="7">
-        <f>DEC2HEX(HEX2DEC(B20)+1)</f>
+    <row r="21" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A21" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B21" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C21" s="2"/>
@@ -2844,14 +2930,14 @@
       <c r="J21" s="9"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" t="s" s="26">
+      <c r="M21" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="25"/>
-      <c r="O21" t="s" s="3">
+      <c r="N21" s="38"/>
+      <c r="O21" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="P21" t="s" s="3">
+      <c r="P21" s="3" t="s">
         <v>104</v>
       </c>
       <c r="Q21" s="2"/>
@@ -2861,13 +2947,13 @@
       <c r="U21" s="2"/>
       <c r="V21" s="6"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="24">
-        <f>HEX2BIN(B22)</f>
-        <v>4</v>
-      </c>
-      <c r="B22" s="7">
-        <f>DEC2HEX(HEX2DEC(B21)+1)</f>
+    <row r="22" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A22" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C22" s="7">
@@ -2888,22 +2974,22 @@
       <c r="H22" s="7">
         <v>0</v>
       </c>
-      <c r="I22" s="27"/>
-      <c r="J22" t="s" s="11">
+      <c r="I22" s="25"/>
+      <c r="J22" s="11" t="s">
         <v>105</v>
       </c>
       <c r="K22" s="12">
         <v>402000</v>
       </c>
       <c r="L22" s="2"/>
-      <c r="M22" t="s" s="26">
+      <c r="M22" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="N22" s="25"/>
-      <c r="O22" t="s" s="3">
+      <c r="N22" s="38"/>
+      <c r="O22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P22" t="s" s="3">
+      <c r="P22" s="3" t="s">
         <v>108</v>
       </c>
       <c r="Q22" s="2"/>
@@ -2913,13 +2999,13 @@
       <c r="U22" s="2"/>
       <c r="V22" s="6"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="24">
-        <f>HEX2BIN(B23)</f>
-        <v>5</v>
-      </c>
-      <c r="B23" s="7">
-        <f>DEC2HEX(HEX2DEC(B22)+1)</f>
+    <row r="23" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A23" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="B23" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="C23" s="7">
@@ -2957,13 +3043,13 @@
       <c r="U23" s="2"/>
       <c r="V23" s="6"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="24">
-        <f>HEX2BIN(B24)</f>
-        <v>6</v>
-      </c>
-      <c r="B24" s="7">
-        <f>DEC2HEX(HEX2DEC(B23)+1)</f>
+    <row r="24" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A24" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="B24" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="C24" s="2"/>
@@ -2976,12 +3062,12 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" t="s" s="3">
+      <c r="M24" s="3" t="s">
         <v>109</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" t="s" s="3">
+      <c r="P24" s="3" t="s">
         <v>110</v>
       </c>
       <c r="Q24" s="2"/>
@@ -2991,13 +3077,13 @@
       <c r="U24" s="2"/>
       <c r="V24" s="6"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="24">
-        <f>HEX2BIN(B25)</f>
-        <v>7</v>
-      </c>
-      <c r="B25" s="7">
-        <f>DEC2HEX(HEX2DEC(B24)+1)</f>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A25" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="B25" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C25" s="2"/>
@@ -3010,12 +3096,12 @@
       <c r="J25" s="9"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" t="s" s="3">
+      <c r="M25" s="3" t="s">
         <v>111</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" t="s" s="3">
+      <c r="P25" s="3" t="s">
         <v>112</v>
       </c>
       <c r="Q25" s="2"/>
@@ -3025,13 +3111,13 @@
       <c r="U25" s="2"/>
       <c r="V25" s="6"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="24">
-        <f>HEX2BIN(B26)</f>
-        <v>8</v>
-      </c>
-      <c r="B26" s="7">
-        <f>DEC2HEX(HEX2DEC(B25)+1)</f>
+    <row r="26" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A26" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="B26" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C26" s="7">
@@ -3052,20 +3138,20 @@
       <c r="H26" s="7">
         <v>0</v>
       </c>
-      <c r="I26" s="27"/>
-      <c r="J26" t="s" s="11">
+      <c r="I26" s="25"/>
+      <c r="J26" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="K26" t="s" s="28">
+      <c r="K26" s="26" t="s">
         <v>114</v>
       </c>
       <c r="L26" s="2"/>
-      <c r="M26" t="s" s="3">
+      <c r="M26" s="3" t="s">
         <v>115</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" t="s" s="3">
+      <c r="P26" s="3" t="s">
         <v>116</v>
       </c>
       <c r="Q26" s="2"/>
@@ -3075,13 +3161,13 @@
       <c r="U26" s="2"/>
       <c r="V26" s="6"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="24">
-        <f>HEX2BIN(B27)</f>
-        <v>9</v>
-      </c>
-      <c r="B27" s="7">
-        <f>DEC2HEX(HEX2DEC(B26)+1)</f>
+    <row r="27" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A27" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+      <c r="B27" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="C27" s="2"/>
@@ -3094,12 +3180,12 @@
       <c r="J27" s="20"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" t="s" s="3">
+      <c r="M27" s="3" t="s">
         <v>117</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" t="s" s="3">
+      <c r="P27" s="3" t="s">
         <v>118</v>
       </c>
       <c r="Q27" s="2"/>
@@ -3109,14 +3195,14 @@
       <c r="U27" s="2"/>
       <c r="V27" s="6"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="24">
-        <f>HEX2BIN(B28)</f>
-        <v>10</v>
-      </c>
-      <c r="B28" s="7">
-        <f>DEC2HEX(HEX2DEC(B27)+1)</f>
-        <v>10</v>
+    <row r="28" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A28" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+      <c r="B28" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>A</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3128,12 +3214,12 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" t="s" s="3">
+      <c r="M28" s="3" t="s">
         <v>119</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="P28" t="s" s="3">
+      <c r="P28" s="3" t="s">
         <v>120</v>
       </c>
       <c r="Q28" s="2"/>
@@ -3143,14 +3229,14 @@
       <c r="U28" s="2"/>
       <c r="V28" s="6"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="24">
-        <f>HEX2BIN(B29)</f>
-        <v>11</v>
-      </c>
-      <c r="B29" s="7">
-        <f>DEC2HEX(HEX2DEC(B28)+1)</f>
-        <v>11</v>
+    <row r="29" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A29" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+      <c r="B29" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>B</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3162,14 +3248,14 @@
       <c r="J29" s="9"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" t="s" s="3">
+      <c r="M29" s="3" t="s">
         <v>121</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" t="s" s="3">
+      <c r="O29" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="P29" t="s" s="3">
+      <c r="P29" s="3" t="s">
         <v>123</v>
       </c>
       <c r="Q29" s="2"/>
@@ -3179,14 +3265,14 @@
       <c r="U29" s="2"/>
       <c r="V29" s="6"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="24">
-        <f>HEX2BIN(B30)</f>
-        <v>12</v>
-      </c>
-      <c r="B30" s="7">
-        <f>DEC2HEX(HEX2DEC(B29)+1)</f>
-        <v>12</v>
+    <row r="30" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A30" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="B30" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
       </c>
       <c r="C30" s="7">
         <v>1</v>
@@ -3206,20 +3292,20 @@
       <c r="H30" s="7">
         <v>0</v>
       </c>
-      <c r="I30" s="27"/>
-      <c r="J30" t="s" s="11">
+      <c r="I30" s="25"/>
+      <c r="J30" s="11" t="s">
         <v>124</v>
       </c>
       <c r="K30" s="12">
         <v>200000</v>
       </c>
       <c r="L30" s="2"/>
-      <c r="M30" t="s" s="3">
+      <c r="M30" s="3" t="s">
         <v>125</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" t="s" s="3">
+      <c r="P30" s="3" t="s">
         <v>126</v>
       </c>
       <c r="Q30" s="2"/>
@@ -3229,14 +3315,14 @@
       <c r="U30" s="2"/>
       <c r="V30" s="6"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="24">
-        <f>HEX2BIN(B31)</f>
-        <v>13</v>
-      </c>
-      <c r="B31" s="7">
-        <f>DEC2HEX(HEX2DEC(B30)+1)</f>
-        <v>13</v>
+    <row r="31" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A31" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+      <c r="B31" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3248,12 +3334,12 @@
       <c r="J31" s="20"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" t="s" s="3">
+      <c r="M31" s="3" t="s">
         <v>127</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" t="s" s="3">
+      <c r="P31" s="3" t="s">
         <v>128</v>
       </c>
       <c r="Q31" s="2"/>
@@ -3263,14 +3349,14 @@
       <c r="U31" s="2"/>
       <c r="V31" s="6"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="24">
-        <f>HEX2BIN(B32)</f>
-        <v>14</v>
-      </c>
-      <c r="B32" s="7">
-        <f>DEC2HEX(HEX2DEC(B31)+1)</f>
-        <v>14</v>
+    <row r="32" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A32" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="B32" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3282,12 +3368,12 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" t="s" s="3">
+      <c r="M32" s="3" t="s">
         <v>129</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" t="s" s="3">
+      <c r="P32" s="3" t="s">
         <v>130</v>
       </c>
       <c r="Q32" s="2"/>
@@ -3297,14 +3383,14 @@
       <c r="U32" s="2"/>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="24">
-        <f>HEX2BIN(B33)</f>
-        <v>15</v>
-      </c>
-      <c r="B33" s="7">
-        <f>DEC2HEX(HEX2DEC(B32)+1)</f>
-        <v>15</v>
+    <row r="33" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A33" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+      <c r="B33" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3316,12 +3402,12 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" t="s" s="3">
+      <c r="M33" s="3" t="s">
         <v>131</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" t="s" s="3">
+      <c r="P33" s="3" t="s">
         <v>132</v>
       </c>
       <c r="Q33" s="2"/>
@@ -3331,14 +3417,14 @@
       <c r="U33" s="2"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="24">
-        <f>HEX2BIN(B34)</f>
-        <v>16</v>
-      </c>
-      <c r="B34" s="7">
-        <f>DEC2HEX(HEX2DEC(B33)+1)</f>
-        <v>16</v>
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A34" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="B34" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="C34" s="22">
         <v>0</v>
@@ -3359,19 +3445,19 @@
         <v>10001</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" t="s" s="3">
+      <c r="J34" s="39" t="s">
         <v>133</v>
       </c>
       <c r="K34" s="7">
         <v>18088</v>
       </c>
       <c r="L34" s="2"/>
-      <c r="M34" t="s" s="3">
+      <c r="M34" s="3" t="s">
         <v>134</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" t="s" s="3">
+      <c r="P34" s="3" t="s">
         <v>135</v>
       </c>
       <c r="Q34" s="2"/>
@@ -3381,14 +3467,14 @@
       <c r="U34" s="2"/>
       <c r="V34" s="6"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="24">
-        <f>HEX2BIN(B35)</f>
-        <v>17</v>
-      </c>
-      <c r="B35" s="7">
-        <f>DEC2HEX(HEX2DEC(B34)+1)</f>
-        <v>17</v>
+    <row r="35" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A35" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10001</v>
+      </c>
+      <c r="B35" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="C35" s="22">
         <v>0</v>
@@ -3425,14 +3511,14 @@
       <c r="U35" s="2"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="24">
-        <f>HEX2BIN(B36)</f>
-        <v>18</v>
-      </c>
-      <c r="B36" s="7">
-        <f>DEC2HEX(HEX2DEC(B35)+1)</f>
-        <v>18</v>
+    <row r="36" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A36" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10010</v>
+      </c>
+      <c r="B36" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3455,14 +3541,14 @@
       <c r="U36" s="2"/>
       <c r="V36" s="6"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="24">
-        <f>HEX2BIN(B37)</f>
-        <v>19</v>
-      </c>
-      <c r="B37" s="7">
-        <f>DEC2HEX(HEX2DEC(B36)+1)</f>
-        <v>19</v>
+    <row r="37" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A37" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10011</v>
+      </c>
+      <c r="B37" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3485,14 +3571,14 @@
       <c r="U37" s="2"/>
       <c r="V37" s="6"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="24">
-        <f>HEX2BIN(B38)</f>
-        <v>20</v>
-      </c>
-      <c r="B38" s="7">
-        <f>DEC2HEX(HEX2DEC(B37)+1)</f>
-        <v>20</v>
+    <row r="38" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A38" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10100</v>
+      </c>
+      <c r="B38" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="C38" s="22">
         <v>0</v>
@@ -3513,10 +3599,10 @@
         <v>10101</v>
       </c>
       <c r="I38" s="2"/>
-      <c r="J38" t="s" s="3">
+      <c r="J38" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="K38" t="s" s="3">
+      <c r="K38" s="3" t="s">
         <v>137</v>
       </c>
       <c r="L38" s="2"/>
@@ -3531,14 +3617,14 @@
       <c r="U38" s="2"/>
       <c r="V38" s="6"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="24">
-        <f>HEX2BIN(B39)</f>
-        <v>21</v>
-      </c>
-      <c r="B39" s="7">
-        <f>DEC2HEX(HEX2DEC(B38)+1)</f>
-        <v>21</v>
+    <row r="39" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A39" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10101</v>
+      </c>
+      <c r="B39" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="C39" s="22">
         <v>0</v>
@@ -3575,14 +3661,14 @@
       <c r="U39" s="2"/>
       <c r="V39" s="6"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="24">
-        <f>HEX2BIN(B40)</f>
-        <v>22</v>
-      </c>
-      <c r="B40" s="7">
-        <f>DEC2HEX(HEX2DEC(B39)+1)</f>
-        <v>22</v>
+    <row r="40" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A40" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10110</v>
+      </c>
+      <c r="B40" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3605,14 +3691,14 @@
       <c r="U40" s="2"/>
       <c r="V40" s="6"/>
     </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="24">
-        <f>HEX2BIN(B41)</f>
-        <v>23</v>
-      </c>
-      <c r="B41" s="7">
-        <f>DEC2HEX(HEX2DEC(B40)+1)</f>
-        <v>23</v>
+    <row r="41" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A41" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>10111</v>
+      </c>
+      <c r="B41" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3635,14 +3721,14 @@
       <c r="U41" s="2"/>
       <c r="V41" s="6"/>
     </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="24">
-        <f>HEX2BIN(B42)</f>
-        <v>24</v>
-      </c>
-      <c r="B42" s="7">
-        <f>DEC2HEX(HEX2DEC(B41)+1)</f>
-        <v>24</v>
+    <row r="42" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A42" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11000</v>
+      </c>
+      <c r="B42" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="C42" s="22">
         <v>0</v>
@@ -3662,8 +3748,8 @@
       <c r="H42" s="7">
         <v>0</v>
       </c>
-      <c r="I42" s="27"/>
-      <c r="J42" t="s" s="11">
+      <c r="I42" s="25"/>
+      <c r="J42" s="11" t="s">
         <v>11</v>
       </c>
       <c r="K42" s="12">
@@ -3681,14 +3767,14 @@
       <c r="U42" s="2"/>
       <c r="V42" s="6"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="24">
-        <f>HEX2BIN(B43)</f>
-        <v>25</v>
-      </c>
-      <c r="B43" s="7">
-        <f>DEC2HEX(HEX2DEC(B42)+1)</f>
-        <v>25</v>
+    <row r="43" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A43" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11001</v>
+      </c>
+      <c r="B43" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -3711,14 +3797,14 @@
       <c r="U43" s="2"/>
       <c r="V43" s="6"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="24">
-        <f>HEX2BIN(B44)</f>
-        <v>26</v>
-      </c>
-      <c r="B44" s="7">
-        <f>DEC2HEX(HEX2DEC(B43)+1)</f>
-        <v>26</v>
+    <row r="44" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A44" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11010</v>
+      </c>
+      <c r="B44" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1A</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3741,14 +3827,14 @@
       <c r="U44" s="2"/>
       <c r="V44" s="6"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="24">
-        <f>HEX2BIN(B45)</f>
-        <v>27</v>
-      </c>
-      <c r="B45" s="7">
-        <f>DEC2HEX(HEX2DEC(B44)+1)</f>
-        <v>27</v>
+    <row r="45" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A45" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11011</v>
+      </c>
+      <c r="B45" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1B</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3771,14 +3857,14 @@
       <c r="U45" s="2"/>
       <c r="V45" s="6"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="24">
-        <f>HEX2BIN(B46)</f>
-        <v>28</v>
-      </c>
-      <c r="B46" s="7">
-        <f>DEC2HEX(HEX2DEC(B45)+1)</f>
-        <v>28</v>
+    <row r="46" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A46" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11100</v>
+      </c>
+      <c r="B46" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1C</v>
       </c>
       <c r="C46" s="22">
         <v>101</v>
@@ -3798,11 +3884,11 @@
       <c r="H46" s="7">
         <v>0</v>
       </c>
-      <c r="I46" s="27"/>
-      <c r="J46" t="s" s="11">
+      <c r="I46" s="25"/>
+      <c r="J46" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K46" t="s" s="28">
+      <c r="K46" s="26" t="s">
         <v>138</v>
       </c>
       <c r="L46" s="2"/>
@@ -3817,14 +3903,14 @@
       <c r="U46" s="2"/>
       <c r="V46" s="6"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="24">
-        <f>HEX2BIN(B47)</f>
-        <v>29</v>
-      </c>
-      <c r="B47" s="7">
-        <f>DEC2HEX(HEX2DEC(B46)+1)</f>
-        <v>29</v>
+    <row r="47" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A47" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11101</v>
+      </c>
+      <c r="B47" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1D</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3847,14 +3933,14 @@
       <c r="U47" s="2"/>
       <c r="V47" s="6"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="24">
-        <f>HEX2BIN(B48)</f>
-        <v>30</v>
-      </c>
-      <c r="B48" s="7">
-        <f>DEC2HEX(HEX2DEC(B47)+1)</f>
-        <v>30</v>
+    <row r="48" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A48" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11110</v>
+      </c>
+      <c r="B48" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1E</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3877,14 +3963,14 @@
       <c r="U48" s="2"/>
       <c r="V48" s="6"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="24">
-        <f>HEX2BIN(B49)</f>
-        <v>31</v>
-      </c>
-      <c r="B49" s="7">
-        <f>DEC2HEX(HEX2DEC(B48)+1)</f>
-        <v>31</v>
+    <row r="49" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A49" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>11111</v>
+      </c>
+      <c r="B49" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>1F</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3907,14 +3993,14 @@
       <c r="U49" s="2"/>
       <c r="V49" s="6"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="24">
-        <f>HEX2BIN(B50)</f>
-        <v>32</v>
-      </c>
-      <c r="B50" s="7">
-        <f>DEC2HEX(HEX2DEC(B49)+1)</f>
-        <v>32</v>
+    <row r="50" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A50" s="24" t="str">
+        <f t="shared" ref="A50:A81" si="2">HEX2BIN(B50)</f>
+        <v>100000</v>
+      </c>
+      <c r="B50" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="C50" s="7">
         <v>1</v>
@@ -3934,8 +4020,8 @@
       <c r="H50" s="7">
         <v>100001</v>
       </c>
-      <c r="I50" s="27"/>
-      <c r="J50" t="s" s="11">
+      <c r="I50" s="25"/>
+      <c r="J50" s="11" t="s">
         <v>47</v>
       </c>
       <c r="K50" s="12">
@@ -3953,14 +4039,14 @@
       <c r="U50" s="2"/>
       <c r="V50" s="6"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="24">
-        <f>HEX2BIN(B51)</f>
-        <v>33</v>
-      </c>
-      <c r="B51" s="7">
-        <f>DEC2HEX(HEX2DEC(B50)+1)</f>
-        <v>33</v>
+    <row r="51" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A51" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100001</v>
+      </c>
+      <c r="B51" s="7" t="str">
+        <f t="shared" ref="B51:B82" si="3">DEC2HEX(HEX2DEC(B50)+1)</f>
+        <v>21</v>
       </c>
       <c r="C51" s="7">
         <v>110</v>
@@ -3982,7 +4068,7 @@
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="20"/>
-      <c r="K51" t="s" s="3">
+      <c r="K51" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L51" s="2"/>
@@ -3997,14 +4083,14 @@
       <c r="U51" s="2"/>
       <c r="V51" s="6"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="24">
-        <f>HEX2BIN(B52)</f>
-        <v>34</v>
-      </c>
-      <c r="B52" s="7">
-        <f>DEC2HEX(HEX2DEC(B51)+1)</f>
-        <v>34</v>
+    <row r="52" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A52" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100010</v>
+      </c>
+      <c r="B52" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>22</v>
       </c>
       <c r="C52" s="7">
         <v>0</v>
@@ -4026,7 +4112,7 @@
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
-      <c r="K52" t="s" s="3">
+      <c r="K52" s="3" t="s">
         <v>140</v>
       </c>
       <c r="L52" s="2"/>
@@ -4041,14 +4127,14 @@
       <c r="U52" s="2"/>
       <c r="V52" s="6"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="24">
-        <f>HEX2BIN(B53)</f>
-        <v>35</v>
-      </c>
-      <c r="B53" s="7">
-        <f>DEC2HEX(HEX2DEC(B52)+1)</f>
-        <v>35</v>
+    <row r="53" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A53" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100011</v>
+      </c>
+      <c r="B53" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>23</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4071,14 +4157,14 @@
       <c r="U53" s="2"/>
       <c r="V53" s="6"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="24">
-        <f>HEX2BIN(B54)</f>
-        <v>36</v>
-      </c>
-      <c r="B54" s="7">
-        <f>DEC2HEX(HEX2DEC(B53)+1)</f>
-        <v>36</v>
+    <row r="54" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A54" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100100</v>
+      </c>
+      <c r="B54" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>24</v>
       </c>
       <c r="C54" s="7">
         <v>1</v>
@@ -4099,7 +4185,7 @@
         <v>100101</v>
       </c>
       <c r="I54" s="2"/>
-      <c r="J54" t="s" s="29">
+      <c r="J54" s="27" t="s">
         <v>33</v>
       </c>
       <c r="K54" s="12">
@@ -4117,14 +4203,14 @@
       <c r="U54" s="2"/>
       <c r="V54" s="6"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="24">
-        <f>HEX2BIN(B55)</f>
-        <v>37</v>
-      </c>
-      <c r="B55" s="7">
-        <f>DEC2HEX(HEX2DEC(B54)+1)</f>
-        <v>37</v>
+    <row r="55" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A55" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100101</v>
+      </c>
+      <c r="B55" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
       <c r="C55" s="7">
         <v>100</v>
@@ -4161,14 +4247,14 @@
       <c r="U55" s="2"/>
       <c r="V55" s="6"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="24">
-        <f>HEX2BIN(B56)</f>
-        <v>38</v>
-      </c>
-      <c r="B56" s="7">
-        <f>DEC2HEX(HEX2DEC(B55)+1)</f>
-        <v>38</v>
+    <row r="56" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A56" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100110</v>
+      </c>
+      <c r="B56" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>26</v>
       </c>
       <c r="C56" s="7">
         <v>0</v>
@@ -4190,7 +4276,7 @@
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="2"/>
-      <c r="K56" t="s" s="3">
+      <c r="K56" s="3" t="s">
         <v>140</v>
       </c>
       <c r="L56" s="2"/>
@@ -4205,14 +4291,14 @@
       <c r="U56" s="2"/>
       <c r="V56" s="6"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="24">
-        <f>HEX2BIN(B57)</f>
-        <v>39</v>
-      </c>
-      <c r="B57" s="7">
-        <f>DEC2HEX(HEX2DEC(B56)+1)</f>
-        <v>39</v>
+    <row r="57" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A57" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>100111</v>
+      </c>
+      <c r="B57" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4235,14 +4321,14 @@
       <c r="U57" s="2"/>
       <c r="V57" s="6"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="24">
-        <f>HEX2BIN(B58)</f>
-        <v>40</v>
-      </c>
-      <c r="B58" s="7">
-        <f>DEC2HEX(HEX2DEC(B57)+1)</f>
-        <v>40</v>
+    <row r="58" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A58" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101000</v>
+      </c>
+      <c r="B58" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>28</v>
       </c>
       <c r="C58" s="22">
         <v>1</v>
@@ -4263,7 +4349,7 @@
         <v>101001</v>
       </c>
       <c r="I58" s="2"/>
-      <c r="J58" t="s" s="3">
+      <c r="J58" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K58" s="2"/>
@@ -4279,14 +4365,14 @@
       <c r="U58" s="2"/>
       <c r="V58" s="6"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="24">
-        <f>HEX2BIN(B59)</f>
-        <v>41</v>
-      </c>
-      <c r="B59" s="7">
-        <f>DEC2HEX(HEX2DEC(B58)+1)</f>
-        <v>41</v>
+    <row r="59" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A59" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101001</v>
+      </c>
+      <c r="B59" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>29</v>
       </c>
       <c r="C59" s="22">
         <v>0</v>
@@ -4321,14 +4407,14 @@
       <c r="U59" s="2"/>
       <c r="V59" s="6"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="24">
-        <f>HEX2BIN(B60)</f>
-        <v>42</v>
-      </c>
-      <c r="B60" s="7">
-        <f>DEC2HEX(HEX2DEC(B59)+1)</f>
-        <v>42</v>
+    <row r="60" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A60" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101010</v>
+      </c>
+      <c r="B60" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2A</v>
       </c>
       <c r="C60" s="22">
         <v>0</v>
@@ -4363,14 +4449,14 @@
       <c r="U60" s="2"/>
       <c r="V60" s="6"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="24">
-        <f>HEX2BIN(B61)</f>
-        <v>43</v>
-      </c>
-      <c r="B61" s="7">
-        <f>DEC2HEX(HEX2DEC(B60)+1)</f>
-        <v>43</v>
+    <row r="61" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A61" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101011</v>
+      </c>
+      <c r="B61" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2B</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4393,14 +4479,14 @@
       <c r="U61" s="2"/>
       <c r="V61" s="6"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="24">
-        <f>HEX2BIN(B62)</f>
-        <v>44</v>
-      </c>
-      <c r="B62" s="7">
-        <f>DEC2HEX(HEX2DEC(B61)+1)</f>
-        <v>44</v>
+    <row r="62" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A62" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101100</v>
+      </c>
+      <c r="B62" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2C</v>
       </c>
       <c r="C62" s="22">
         <v>1</v>
@@ -4421,7 +4507,7 @@
         <v>101101</v>
       </c>
       <c r="I62" s="2"/>
-      <c r="J62" t="s" s="3">
+      <c r="J62" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K62" s="2"/>
@@ -4437,14 +4523,14 @@
       <c r="U62" s="2"/>
       <c r="V62" s="6"/>
     </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="24">
-        <f>HEX2BIN(B63)</f>
-        <v>45</v>
-      </c>
-      <c r="B63" s="7">
-        <f>DEC2HEX(HEX2DEC(B62)+1)</f>
-        <v>45</v>
+    <row r="63" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A63" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101101</v>
+      </c>
+      <c r="B63" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2D</v>
       </c>
       <c r="C63" s="22">
         <v>0</v>
@@ -4479,14 +4565,14 @@
       <c r="U63" s="2"/>
       <c r="V63" s="6"/>
     </row>
-    <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="24">
-        <f>HEX2BIN(B64)</f>
-        <v>46</v>
-      </c>
-      <c r="B64" s="7">
-        <f>DEC2HEX(HEX2DEC(B63)+1)</f>
-        <v>46</v>
+    <row r="64" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A64" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101110</v>
+      </c>
+      <c r="B64" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2E</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4509,14 +4595,14 @@
       <c r="U64" s="2"/>
       <c r="V64" s="6"/>
     </row>
-    <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="24">
-        <f>HEX2BIN(B65)</f>
-        <v>47</v>
-      </c>
-      <c r="B65" s="7">
-        <f>DEC2HEX(HEX2DEC(B64)+1)</f>
-        <v>47</v>
+    <row r="65" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A65" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>101111</v>
+      </c>
+      <c r="B65" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>2F</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4539,14 +4625,14 @@
       <c r="U65" s="2"/>
       <c r="V65" s="6"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="24">
-        <f>HEX2BIN(B66)</f>
-        <v>48</v>
-      </c>
-      <c r="B66" s="7">
-        <f>DEC2HEX(HEX2DEC(B65)+1)</f>
-        <v>48</v>
+    <row r="66" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A66" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110000</v>
+      </c>
+      <c r="B66" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>30</v>
       </c>
       <c r="C66" s="22">
         <v>0</v>
@@ -4567,7 +4653,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="2"/>
-      <c r="J66" t="s" s="13">
+      <c r="J66" s="13" t="s">
         <v>35</v>
       </c>
       <c r="K66" s="7">
@@ -4585,14 +4671,14 @@
       <c r="U66" s="2"/>
       <c r="V66" s="6"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="24">
-        <f>HEX2BIN(B67)</f>
-        <v>49</v>
-      </c>
-      <c r="B67" s="7">
-        <f>DEC2HEX(HEX2DEC(B66)+1)</f>
-        <v>49</v>
+    <row r="67" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A67" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110001</v>
+      </c>
+      <c r="B67" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>31</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4615,14 +4701,14 @@
       <c r="U67" s="2"/>
       <c r="V67" s="6"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="24">
-        <f>HEX2BIN(B68)</f>
-        <v>50</v>
-      </c>
-      <c r="B68" s="7">
-        <f>DEC2HEX(HEX2DEC(B67)+1)</f>
-        <v>50</v>
+    <row r="68" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A68" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110010</v>
+      </c>
+      <c r="B68" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>32</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4645,14 +4731,14 @@
       <c r="U68" s="2"/>
       <c r="V68" s="6"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="24">
-        <f>HEX2BIN(B69)</f>
-        <v>51</v>
-      </c>
-      <c r="B69" s="7">
-        <f>DEC2HEX(HEX2DEC(B68)+1)</f>
-        <v>51</v>
+    <row r="69" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A69" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110011</v>
+      </c>
+      <c r="B69" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>33</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4661,7 +4747,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="J69" s="30"/>
+      <c r="J69" s="28"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
@@ -4675,14 +4761,14 @@
       <c r="U69" s="2"/>
       <c r="V69" s="6"/>
     </row>
-    <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="24">
-        <f>HEX2BIN(B70)</f>
-        <v>52</v>
-      </c>
-      <c r="B70" s="7">
-        <f>DEC2HEX(HEX2DEC(B69)+1)</f>
-        <v>52</v>
+    <row r="70" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A70" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110100</v>
+      </c>
+      <c r="B70" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>34</v>
       </c>
       <c r="C70" s="22">
         <v>0</v>
@@ -4702,11 +4788,11 @@
       <c r="H70" s="7">
         <v>0</v>
       </c>
-      <c r="I70" s="31"/>
-      <c r="J70" t="s" s="32">
+      <c r="I70" s="29"/>
+      <c r="J70" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="K70" s="33">
+      <c r="K70" s="31">
         <v>140000</v>
       </c>
       <c r="L70" s="2"/>
@@ -4721,14 +4807,14 @@
       <c r="U70" s="2"/>
       <c r="V70" s="6"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="24">
-        <f>HEX2BIN(B71)</f>
-        <v>53</v>
-      </c>
-      <c r="B71" s="7">
-        <f>DEC2HEX(HEX2DEC(B70)+1)</f>
-        <v>53</v>
+    <row r="71" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A71" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110101</v>
+      </c>
+      <c r="B71" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -4737,7 +4823,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
-      <c r="J71" s="34"/>
+      <c r="J71" s="32"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
@@ -4751,14 +4837,14 @@
       <c r="U71" s="2"/>
       <c r="V71" s="6"/>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="24">
-        <f>HEX2BIN(B72)</f>
-        <v>54</v>
-      </c>
-      <c r="B72" s="7">
-        <f>DEC2HEX(HEX2DEC(B71)+1)</f>
-        <v>54</v>
+    <row r="72" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A72" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110110</v>
+      </c>
+      <c r="B72" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>36</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
@@ -4781,14 +4867,14 @@
       <c r="U72" s="2"/>
       <c r="V72" s="6"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="24">
-        <f>HEX2BIN(B73)</f>
-        <v>55</v>
-      </c>
-      <c r="B73" s="7">
-        <f>DEC2HEX(HEX2DEC(B72)+1)</f>
-        <v>55</v>
+    <row r="73" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A73" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>110111</v>
+      </c>
+      <c r="B73" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -4811,14 +4897,14 @@
       <c r="U73" s="2"/>
       <c r="V73" s="6"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="24">
-        <f>HEX2BIN(B74)</f>
-        <v>56</v>
-      </c>
-      <c r="B74" s="7">
-        <f>DEC2HEX(HEX2DEC(B73)+1)</f>
-        <v>56</v>
+    <row r="74" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A74" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111000</v>
+      </c>
+      <c r="B74" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>38</v>
       </c>
       <c r="C74" s="22">
         <v>0</v>
@@ -4839,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="2"/>
-      <c r="J74" t="s" s="13">
+      <c r="J74" s="13" t="s">
         <v>142</v>
       </c>
       <c r="K74" s="7">
@@ -4857,14 +4943,14 @@
       <c r="U74" s="2"/>
       <c r="V74" s="6"/>
     </row>
-    <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="24">
-        <f>HEX2BIN(B75)</f>
-        <v>57</v>
-      </c>
-      <c r="B75" s="7">
-        <f>DEC2HEX(HEX2DEC(B74)+1)</f>
-        <v>57</v>
+    <row r="75" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A75" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111001</v>
+      </c>
+      <c r="B75" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>39</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -4887,14 +4973,14 @@
       <c r="U75" s="2"/>
       <c r="V75" s="6"/>
     </row>
-    <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="24">
-        <f>HEX2BIN(B76)</f>
-        <v>58</v>
-      </c>
-      <c r="B76" s="7">
-        <f>DEC2HEX(HEX2DEC(B75)+1)</f>
-        <v>58</v>
+    <row r="76" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A76" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111010</v>
+      </c>
+      <c r="B76" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3A</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
@@ -4917,14 +5003,14 @@
       <c r="U76" s="2"/>
       <c r="V76" s="6"/>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="24">
-        <f>HEX2BIN(B77)</f>
-        <v>59</v>
-      </c>
-      <c r="B77" s="7">
-        <f>DEC2HEX(HEX2DEC(B76)+1)</f>
-        <v>59</v>
+    <row r="77" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A77" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111011</v>
+      </c>
+      <c r="B77" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3B</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
@@ -4947,14 +5033,14 @@
       <c r="U77" s="2"/>
       <c r="V77" s="6"/>
     </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="24">
-        <f>HEX2BIN(B78)</f>
-        <v>60</v>
-      </c>
-      <c r="B78" s="7">
-        <f>DEC2HEX(HEX2DEC(B77)+1)</f>
-        <v>60</v>
+    <row r="78" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A78" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111100</v>
+      </c>
+      <c r="B78" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3C</v>
       </c>
       <c r="C78" s="22">
         <v>0</v>
@@ -4974,8 +5060,8 @@
       <c r="H78" s="22">
         <v>0</v>
       </c>
-      <c r="I78" s="27"/>
-      <c r="J78" t="s" s="11">
+      <c r="I78" s="25"/>
+      <c r="J78" s="11" t="s">
         <v>143</v>
       </c>
       <c r="K78" s="12">
@@ -4993,21 +5079,21 @@
       <c r="U78" s="2"/>
       <c r="V78" s="6"/>
     </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="24">
-        <f>HEX2BIN(B79)</f>
-        <v>61</v>
-      </c>
-      <c r="B79" s="7">
-        <f>DEC2HEX(HEX2DEC(B78)+1)</f>
-        <v>61</v>
-      </c>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="35"/>
+    <row r="79" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A79" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111101</v>
+      </c>
+      <c r="B79" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3D</v>
+      </c>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+      <c r="H79" s="33"/>
       <c r="I79" s="2"/>
       <c r="J79" s="20"/>
       <c r="K79" s="2"/>
@@ -5023,14 +5109,14 @@
       <c r="U79" s="2"/>
       <c r="V79" s="6"/>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="24">
-        <f>HEX2BIN(B80)</f>
-        <v>62</v>
-      </c>
-      <c r="B80" s="7">
-        <f>DEC2HEX(HEX2DEC(B79)+1)</f>
-        <v>62</v>
+    <row r="80" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A80" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111110</v>
+      </c>
+      <c r="B80" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3E</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
@@ -5053,14 +5139,14 @@
       <c r="U80" s="2"/>
       <c r="V80" s="6"/>
     </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="24">
-        <f>HEX2BIN(B81)</f>
-        <v>63</v>
-      </c>
-      <c r="B81" s="7">
-        <f>DEC2HEX(HEX2DEC(B80)+1)</f>
-        <v>63</v>
+    <row r="81" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A81" s="24" t="str">
+        <f t="shared" si="2"/>
+        <v>111111</v>
+      </c>
+      <c r="B81" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>3F</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -5083,14 +5169,14 @@
       <c r="U81" s="2"/>
       <c r="V81" s="6"/>
     </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="24">
-        <f>HEX2BIN(B82)</f>
-        <v>64</v>
-      </c>
-      <c r="B82" s="7">
-        <f>DEC2HEX(HEX2DEC(B81)+1)</f>
-        <v>64</v>
+    <row r="82" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A82" s="24" t="str">
+        <f t="shared" ref="A82:A113" si="4">HEX2BIN(B82)</f>
+        <v>1000000</v>
+      </c>
+      <c r="B82" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>40</v>
       </c>
       <c r="C82" s="22">
         <v>0</v>
@@ -5110,8 +5196,8 @@
       <c r="H82" s="22">
         <v>1000010</v>
       </c>
-      <c r="I82" s="27"/>
-      <c r="J82" t="s" s="11">
+      <c r="I82" s="25"/>
+      <c r="J82" s="11" t="s">
         <v>144</v>
       </c>
       <c r="K82" s="12">
@@ -5129,14 +5215,14 @@
       <c r="U82" s="2"/>
       <c r="V82" s="6"/>
     </row>
-    <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="24">
-        <f>HEX2BIN(B83)</f>
-        <v>65</v>
-      </c>
-      <c r="B83" s="7">
-        <f>DEC2HEX(HEX2DEC(B82)+1)</f>
-        <v>65</v>
+    <row r="83" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A83" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000001</v>
+      </c>
+      <c r="B83" s="7" t="str">
+        <f t="shared" ref="B83:B97" si="5">DEC2HEX(HEX2DEC(B82)+1)</f>
+        <v>41</v>
       </c>
       <c r="C83" s="22">
         <v>0</v>
@@ -5173,14 +5259,14 @@
       <c r="U83" s="2"/>
       <c r="V83" s="6"/>
     </row>
-    <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="24">
-        <f>HEX2BIN(B84)</f>
-        <v>66</v>
-      </c>
-      <c r="B84" s="7">
-        <f>DEC2HEX(HEX2DEC(B83)+1)</f>
-        <v>66</v>
+    <row r="84" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A84" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000010</v>
+      </c>
+      <c r="B84" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>42</v>
       </c>
       <c r="C84" s="22">
         <v>0</v>
@@ -5217,14 +5303,14 @@
       <c r="U84" s="2"/>
       <c r="V84" s="6"/>
     </row>
-    <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="24">
-        <f>HEX2BIN(B85)</f>
-        <v>67</v>
-      </c>
-      <c r="B85" s="7">
-        <f>DEC2HEX(HEX2DEC(B84)+1)</f>
-        <v>67</v>
+    <row r="85" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A85" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000011</v>
+      </c>
+      <c r="B85" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>43</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
@@ -5247,14 +5333,14 @@
       <c r="U85" s="2"/>
       <c r="V85" s="6"/>
     </row>
-    <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="24">
-        <f>HEX2BIN(B86)</f>
-        <v>68</v>
-      </c>
-      <c r="B86" s="7">
-        <f>DEC2HEX(HEX2DEC(B85)+1)</f>
-        <v>68</v>
+    <row r="86" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A86" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000100</v>
+      </c>
+      <c r="B86" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>44</v>
       </c>
       <c r="C86" s="22">
         <v>0</v>
@@ -5274,8 +5360,8 @@
       <c r="H86" s="22">
         <v>0</v>
       </c>
-      <c r="I86" s="27"/>
-      <c r="J86" t="s" s="11">
+      <c r="I86" s="25"/>
+      <c r="J86" s="11" t="s">
         <v>145</v>
       </c>
       <c r="K86" s="12">
@@ -5293,14 +5379,14 @@
       <c r="U86" s="2"/>
       <c r="V86" s="6"/>
     </row>
-    <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="24">
-        <f>HEX2BIN(B87)</f>
-        <v>69</v>
-      </c>
-      <c r="B87" s="7">
-        <f>DEC2HEX(HEX2DEC(B86)+1)</f>
-        <v>69</v>
+    <row r="87" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A87" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000101</v>
+      </c>
+      <c r="B87" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>45</v>
       </c>
       <c r="C87" s="22">
         <v>0</v>
@@ -5337,20 +5423,20 @@
       <c r="U87" s="2"/>
       <c r="V87" s="6"/>
     </row>
-    <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="24">
-        <f>HEX2BIN(B88)</f>
-        <v>70</v>
-      </c>
-      <c r="B88" s="7">
-        <f>DEC2HEX(HEX2DEC(B87)+1)</f>
-        <v>70</v>
-      </c>
-      <c r="C88" s="35"/>
-      <c r="D88" s="35"/>
+    <row r="88" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A88" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000110</v>
+      </c>
+      <c r="B88" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="35"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="33"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -5367,14 +5453,14 @@
       <c r="U88" s="2"/>
       <c r="V88" s="6"/>
     </row>
-    <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="24">
-        <f>HEX2BIN(B89)</f>
-        <v>71</v>
-      </c>
-      <c r="B89" s="7">
-        <f>DEC2HEX(HEX2DEC(B88)+1)</f>
-        <v>71</v>
+    <row r="89" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A89" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1000111</v>
+      </c>
+      <c r="B89" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>47</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -5397,14 +5483,14 @@
       <c r="U89" s="2"/>
       <c r="V89" s="6"/>
     </row>
-    <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="24">
-        <f>HEX2BIN(B90)</f>
-        <v>72</v>
-      </c>
-      <c r="B90" s="7">
-        <f>DEC2HEX(HEX2DEC(B89)+1)</f>
-        <v>72</v>
+    <row r="90" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A90" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001000</v>
+      </c>
+      <c r="B90" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>48</v>
       </c>
       <c r="C90" s="22">
         <v>0</v>
@@ -5425,7 +5511,7 @@
         <v>1001001</v>
       </c>
       <c r="I90" s="2"/>
-      <c r="J90" t="s" s="3">
+      <c r="J90" s="39" t="s">
         <v>146</v>
       </c>
       <c r="K90" s="7">
@@ -5443,14 +5529,14 @@
       <c r="U90" s="2"/>
       <c r="V90" s="6"/>
     </row>
-    <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="24">
-        <f>HEX2BIN(B91)</f>
-        <v>73</v>
-      </c>
-      <c r="B91" s="7">
-        <f>DEC2HEX(HEX2DEC(B90)+1)</f>
-        <v>73</v>
+    <row r="91" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A91" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001001</v>
+      </c>
+      <c r="B91" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>49</v>
       </c>
       <c r="C91" s="22">
         <v>0</v>
@@ -5487,14 +5573,14 @@
       <c r="U91" s="2"/>
       <c r="V91" s="6"/>
     </row>
-    <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="24">
-        <f>HEX2BIN(B92)</f>
-        <v>74</v>
-      </c>
-      <c r="B92" s="7">
-        <f>DEC2HEX(HEX2DEC(B91)+1)</f>
-        <v>74</v>
+    <row r="92" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A92" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001010</v>
+      </c>
+      <c r="B92" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4A</v>
       </c>
       <c r="C92" s="22">
         <v>0</v>
@@ -5531,14 +5617,14 @@
       <c r="U92" s="2"/>
       <c r="V92" s="6"/>
     </row>
-    <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="24">
-        <f>HEX2BIN(B93)</f>
-        <v>75</v>
-      </c>
-      <c r="B93" s="7">
-        <f>DEC2HEX(HEX2DEC(B92)+1)</f>
-        <v>75</v>
+    <row r="93" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A93" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001011</v>
+      </c>
+      <c r="B93" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4B</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
@@ -5561,14 +5647,14 @@
       <c r="U93" s="2"/>
       <c r="V93" s="6"/>
     </row>
-    <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="24">
-        <f>HEX2BIN(B94)</f>
-        <v>76</v>
-      </c>
-      <c r="B94" s="7">
-        <f>DEC2HEX(HEX2DEC(B93)+1)</f>
-        <v>76</v>
+    <row r="94" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A94" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001100</v>
+      </c>
+      <c r="B94" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4C</v>
       </c>
       <c r="C94" s="22">
         <v>0</v>
@@ -5589,7 +5675,7 @@
         <v>1001101</v>
       </c>
       <c r="I94" s="2"/>
-      <c r="J94" t="s" s="3">
+      <c r="J94" s="39" t="s">
         <v>147</v>
       </c>
       <c r="K94" s="7">
@@ -5607,14 +5693,14 @@
       <c r="U94" s="2"/>
       <c r="V94" s="6"/>
     </row>
-    <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="24">
-        <f>HEX2BIN(B95)</f>
-        <v>77</v>
-      </c>
-      <c r="B95" s="7">
-        <f>DEC2HEX(HEX2DEC(B94)+1)</f>
-        <v>77</v>
+    <row r="95" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A95" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001101</v>
+      </c>
+      <c r="B95" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4D</v>
       </c>
       <c r="C95" s="22">
         <v>0</v>
@@ -5651,14 +5737,14 @@
       <c r="U95" s="2"/>
       <c r="V95" s="6"/>
     </row>
-    <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="24">
-        <f>HEX2BIN(B96)</f>
-        <v>78</v>
-      </c>
-      <c r="B96" s="7">
-        <f>DEC2HEX(HEX2DEC(B95)+1)</f>
-        <v>78</v>
+    <row r="96" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A96" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>1001110</v>
+      </c>
+      <c r="B96" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4E</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -5681,35 +5767,35 @@
       <c r="U96" s="2"/>
       <c r="V96" s="6"/>
     </row>
-    <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="36">
-        <f>HEX2BIN(B97)</f>
-        <v>79</v>
-      </c>
-      <c r="B97" s="7">
-        <f>DEC2HEX(HEX2DEC(B96)+1)</f>
-        <v>79</v>
-      </c>
-      <c r="C97" s="37"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="37"/>
-      <c r="I97" s="37"/>
-      <c r="J97" s="37"/>
-      <c r="K97" s="37"/>
-      <c r="L97" s="37"/>
-      <c r="M97" s="37"/>
-      <c r="N97" s="37"/>
-      <c r="O97" s="37"/>
-      <c r="P97" s="37"/>
-      <c r="Q97" s="37"/>
-      <c r="R97" s="37"/>
-      <c r="S97" s="37"/>
-      <c r="T97" s="37"/>
-      <c r="U97" s="37"/>
-      <c r="V97" s="38"/>
+    <row r="97" spans="1:22" ht="15.75" customHeight="1">
+      <c r="A97" s="34" t="str">
+        <f t="shared" si="4"/>
+        <v>1001111</v>
+      </c>
+      <c r="B97" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>4F</v>
+      </c>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="35"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="35"/>
+      <c r="J97" s="35"/>
+      <c r="K97" s="35"/>
+      <c r="L97" s="35"/>
+      <c r="M97" s="35"/>
+      <c r="N97" s="35"/>
+      <c r="O97" s="35"/>
+      <c r="P97" s="35"/>
+      <c r="Q97" s="35"/>
+      <c r="R97" s="35"/>
+      <c r="S97" s="35"/>
+      <c r="T97" s="35"/>
+      <c r="U97" s="35"/>
+      <c r="V97" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5720,7 +5806,7 @@
     <mergeCell ref="M18:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>